<commit_message>
Update investment 1 date display
</commit_message>
<xml_diff>
--- a/semester01/COMP7802B Introduction to financial computing/Assignment 1/Darasirikul_Varis_2020_Assignment 1_Question.xlsx
+++ b/semester01/COMP7802B Introduction to financial computing/Assignment 1/Darasirikul_Varis_2020_Assignment 1_Question.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE937AA3-65A9-604B-ACFA-9BF758BB5A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9167A7-09D7-724F-8054-23A7D42CB3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34260" yWindow="360" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29940" yWindow="-1740" windowWidth="33540" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <definedName name="LastMonthly2">Investment!$F$20</definedName>
     <definedName name="Monthly1">Investment!$B$19</definedName>
     <definedName name="Monthly2">Investment!$F$19</definedName>
+    <definedName name="MonthsCounter">(Investment!$B$21)*12</definedName>
+    <definedName name="October_30__2020">Investment!$A$30</definedName>
     <definedName name="PayOutPeriod1">Investment!$B$21</definedName>
     <definedName name="PayOutPeriod2">Investment!$F$21</definedName>
     <definedName name="rate">Investment!$D$23</definedName>
@@ -50,22 +52,11 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="33">
   <si>
     <t>Payout Amount</t>
   </si>
@@ -299,6 +290,9 @@
   <si>
     <t>Question Requirements</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -907,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1013,9 @@
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="I8" s="27" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
@@ -1173,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>3</v>
@@ -1306,6 +1302,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
+        <f>IF(ROW($A1) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A1)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44134</v>
       </c>
       <c r="B30" s="9">
@@ -1314,6 +1311,10 @@
       <c r="C30" s="9">
         <v>19920.236573710612</v>
       </c>
+      <c r="D30">
+        <f>MonthsCounter</f>
+        <v>84</v>
+      </c>
       <c r="E30" s="7">
         <v>44134</v>
       </c>
@@ -1335,6 +1336,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
+        <f>IF(ROW($A2) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A2)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44165</v>
       </c>
       <c r="B31" s="9">
@@ -1364,6 +1366,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
+        <f>IF(ROW($A3) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A3)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44196</v>
       </c>
       <c r="B32" s="9">
@@ -1393,6 +1396,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
+        <f>IF(ROW($A4) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A4)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44225</v>
       </c>
       <c r="B33" s="9">
@@ -1422,6 +1426,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
+        <f>IF(ROW($A5) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A5)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44253</v>
       </c>
       <c r="B34" s="9">
@@ -1451,6 +1456,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
+        <f>IF(ROW($A6) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A6)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44286</v>
       </c>
       <c r="B35" s="9">
@@ -1480,6 +1486,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
+        <f>IF(ROW($A7) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A7)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44316</v>
       </c>
       <c r="B36" s="9">
@@ -1509,6 +1516,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
+        <f>IF(ROW($A8) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A8)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44347</v>
       </c>
       <c r="B37" s="9">
@@ -1538,6 +1546,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
+        <f>IF(ROW($A9) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A9)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44377</v>
       </c>
       <c r="B38" s="9">
@@ -1567,6 +1576,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
+        <f>IF(ROW($A10) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A10)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44407</v>
       </c>
       <c r="B39" s="9">
@@ -1596,6 +1606,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
+        <f>IF(ROW($A11) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A11)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44439</v>
       </c>
       <c r="B40" s="9">
@@ -1625,6 +1636,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
+        <f>IF(ROW($A12) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A12)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44469</v>
       </c>
       <c r="B41" s="9">
@@ -1654,6 +1666,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
+        <f>IF(ROW($A13) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A13)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44498</v>
       </c>
       <c r="B42" s="9">
@@ -1684,6 +1697,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
+        <f>IF(ROW($A14) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A14)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44530</v>
       </c>
       <c r="B43" s="9">
@@ -1713,6 +1727,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
+        <f>IF(ROW($A15) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A15)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44561</v>
       </c>
       <c r="B44" s="9">
@@ -1742,6 +1757,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
+        <f>IF(ROW($A16) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A16)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44592</v>
       </c>
       <c r="B45" s="9">
@@ -1771,6 +1787,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
+        <f>IF(ROW($A17) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A17)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44620</v>
       </c>
       <c r="B46" s="9">
@@ -1800,6 +1817,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
+        <f>IF(ROW($A18) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A18)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44651</v>
       </c>
       <c r="B47" s="9">
@@ -1829,6 +1847,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
+        <f>IF(ROW($A19) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A19)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44680</v>
       </c>
       <c r="B48" s="9">
@@ -1858,6 +1877,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
+        <f>IF(ROW($A20) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A20)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44712</v>
       </c>
       <c r="B49" s="9">
@@ -1887,6 +1907,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
+        <f>IF(ROW($A21) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A21)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44742</v>
       </c>
       <c r="B50" s="9">
@@ -1916,6 +1937,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
+        <f>IF(ROW($A22) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A22)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44771</v>
       </c>
       <c r="B51" s="9">
@@ -1945,6 +1967,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
+        <f>IF(ROW($A23) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A23)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44804</v>
       </c>
       <c r="B52" s="9">
@@ -1974,6 +1997,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
+        <f>IF(ROW($A24) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A24)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44834</v>
       </c>
       <c r="B53" s="9">
@@ -2003,6 +2027,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
+        <f>IF(ROW($A25) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A25)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44865</v>
       </c>
       <c r="B54" s="9">
@@ -2032,6 +2057,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
+        <f>IF(ROW($A26) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A26)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44895</v>
       </c>
       <c r="B55" s="9">
@@ -2061,6 +2087,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
+        <f>IF(ROW($A27) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A27)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44925</v>
       </c>
       <c r="B56" s="9">
@@ -2090,6 +2117,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
+        <f>IF(ROW($A28) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A28)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44957</v>
       </c>
       <c r="B57" s="9">
@@ -2119,6 +2147,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
+        <f>IF(ROW($A29) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A29)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>44985</v>
       </c>
       <c r="B58" s="9">
@@ -2148,6 +2177,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
+        <f>IF(ROW($A30) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A30)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45016</v>
       </c>
       <c r="B59" s="9">
@@ -2177,6 +2207,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
+        <f>IF(ROW($A31) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A31)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45044</v>
       </c>
       <c r="B60" s="9">
@@ -2206,6 +2237,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
+        <f>IF(ROW($A32) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A32)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45077</v>
       </c>
       <c r="B61" s="9">
@@ -2235,6 +2267,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
+        <f>IF(ROW($A33) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A33)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45107</v>
       </c>
       <c r="B62" s="9">
@@ -2264,6 +2297,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
+        <f>IF(ROW($A34) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A34)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45138</v>
       </c>
       <c r="B63" s="9">
@@ -2284,6 +2318,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
+        <f>IF(ROW($A35) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A35)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45169</v>
       </c>
       <c r="B64" s="9">
@@ -2304,6 +2339,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
+        <f>IF(ROW($A36) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A36)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45198</v>
       </c>
       <c r="B65" s="9">
@@ -2324,6 +2360,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
+        <f>IF(ROW($A37) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A37)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45230</v>
       </c>
       <c r="B66" s="9">
@@ -2344,6 +2381,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
+        <f>IF(ROW($A38) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A38)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45260</v>
       </c>
       <c r="B67" s="9">
@@ -2364,6 +2402,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
+        <f>IF(ROW($A39) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A39)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45289</v>
       </c>
       <c r="B68" s="9">
@@ -2384,6 +2423,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
+        <f>IF(ROW($A40) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A40)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45322</v>
       </c>
       <c r="B69" s="9">
@@ -2404,6 +2444,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
+        <f>IF(ROW($A41) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A41)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45351</v>
       </c>
       <c r="B70" s="9">
@@ -2424,6 +2465,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
+        <f>IF(ROW($A42) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A42)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45379</v>
       </c>
       <c r="B71" s="9">
@@ -2444,6 +2486,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
+        <f>IF(ROW($A43) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A43)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45412</v>
       </c>
       <c r="B72" s="9">
@@ -2464,6 +2507,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
+        <f>IF(ROW($A44) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A44)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45443</v>
       </c>
       <c r="B73" s="9">
@@ -2484,6 +2528,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
+        <f>IF(ROW($A45) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A45)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45471</v>
       </c>
       <c r="B74" s="9">
@@ -2504,6 +2549,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
+        <f>IF(ROW($A46) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A46)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45504</v>
       </c>
       <c r="B75" s="9">
@@ -2524,6 +2570,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
+        <f>IF(ROW($A47) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A47)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45534</v>
       </c>
       <c r="B76" s="9">
@@ -2544,6 +2591,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
+        <f>IF(ROW($A48) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A48)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45565</v>
       </c>
       <c r="B77" s="9">
@@ -2564,6 +2612,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
+        <f>IF(ROW($A49) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A49)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45596</v>
       </c>
       <c r="B78" s="9">
@@ -2584,6 +2633,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
+        <f>IF(ROW($A50) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A50)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45625</v>
       </c>
       <c r="B79" s="9">
@@ -2604,6 +2654,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
+        <f>IF(ROW($A51) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A51)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45657</v>
       </c>
       <c r="B80" s="9">
@@ -2624,6 +2675,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
+        <f>IF(ROW($A52) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A52)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45685</v>
       </c>
       <c r="B81" s="9">
@@ -2644,6 +2696,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
+        <f>IF(ROW($A53) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A53)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45716</v>
       </c>
       <c r="B82" s="9">
@@ -2664,6 +2717,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
+        <f>IF(ROW($A54) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A54)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45747</v>
       </c>
       <c r="B83" s="9">
@@ -2684,6 +2738,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
+        <f>IF(ROW($A55) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A55)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45777</v>
       </c>
       <c r="B84" s="9">
@@ -2704,6 +2759,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
+        <f>IF(ROW($A56) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A56)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45807</v>
       </c>
       <c r="B85" s="9">
@@ -2724,6 +2780,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
+        <f>IF(ROW($A57) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A57)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45838</v>
       </c>
       <c r="B86" s="9">
@@ -2744,6 +2801,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
+        <f>IF(ROW($A58) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A58)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45869</v>
       </c>
       <c r="B87" s="9">
@@ -2764,6 +2822,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
+        <f>IF(ROW($A59) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A59)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45898</v>
       </c>
       <c r="B88" s="9">
@@ -2784,6 +2843,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
+        <f>IF(ROW($A60) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A60)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
         <v>45930</v>
       </c>
       <c r="B89" s="9">
@@ -2803,8 +2863,9 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
-        <v>18</v>
+      <c r="A90" s="7">
+        <f>IF(ROW($A61) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A61)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>45961</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>18</v>
@@ -2823,8 +2884,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
-        <v>18</v>
+      <c r="A91" s="7">
+        <f>IF(ROW($A62) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A62)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>45989</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>18</v>
@@ -2843,8 +2905,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
-        <v>18</v>
+      <c r="A92" s="7">
+        <f>IF(ROW($A63) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A63)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46022</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>18</v>
@@ -2863,8 +2926,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
-        <v>18</v>
+      <c r="A93" s="7">
+        <f>IF(ROW($A64) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A64)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46052</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>18</v>
@@ -2883,8 +2947,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
-        <v>18</v>
+      <c r="A94" s="7">
+        <f>IF(ROW($A65) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A65)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46080</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>18</v>
@@ -2903,8 +2968,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
-        <v>18</v>
+      <c r="A95" s="7">
+        <f>IF(ROW($A66) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A66)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46112</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>18</v>
@@ -2923,8 +2989,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
-        <v>18</v>
+      <c r="A96" s="7">
+        <f>IF(ROW($A67) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A67)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46142</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>18</v>
@@ -2943,8 +3010,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
-        <v>18</v>
+      <c r="A97" s="7">
+        <f>IF(ROW($A68) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A68)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46171</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>18</v>
@@ -2963,8 +3031,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
-        <v>18</v>
+      <c r="A98" s="7">
+        <f>IF(ROW($A69) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A69)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46203</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>18</v>
@@ -2983,8 +3052,9 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
-        <v>18</v>
+      <c r="A99" s="7">
+        <f>IF(ROW($A70) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A70)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46234</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>18</v>
@@ -3003,8 +3073,9 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="7" t="s">
-        <v>18</v>
+      <c r="A100" s="7">
+        <f>IF(ROW($A71) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A71)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46265</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>18</v>
@@ -3023,8 +3094,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
-        <v>18</v>
+      <c r="A101" s="7">
+        <f>IF(ROW($A72) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A72)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46295</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>18</v>
@@ -3043,8 +3115,9 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
-        <v>18</v>
+      <c r="A102" s="7">
+        <f>IF(ROW($A73) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A73)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46325</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>18</v>
@@ -3063,8 +3136,9 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
-        <v>18</v>
+      <c r="A103" s="7">
+        <f>IF(ROW($A74) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A74)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46356</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>18</v>
@@ -3083,8 +3157,9 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
-        <v>18</v>
+      <c r="A104" s="7">
+        <f>IF(ROW($A75) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A75)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46387</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>18</v>
@@ -3103,8 +3178,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
-        <v>18</v>
+      <c r="A105" s="7">
+        <f>IF(ROW($A76) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A76)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46416</v>
       </c>
       <c r="B105" s="9" t="s">
         <v>18</v>
@@ -3123,8 +3199,9 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
-        <v>18</v>
+      <c r="A106" s="7">
+        <f>IF(ROW($A77) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A77)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46444</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>18</v>
@@ -3143,8 +3220,9 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
-        <v>18</v>
+      <c r="A107" s="7">
+        <f>IF(ROW($A78) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A78)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46477</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>18</v>
@@ -3163,8 +3241,9 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
-        <v>18</v>
+      <c r="A108" s="7">
+        <f>IF(ROW($A79) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A79)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46507</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>18</v>
@@ -3183,8 +3262,9 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
-        <v>18</v>
+      <c r="A109" s="7">
+        <f>IF(ROW($A80) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A80)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46538</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>18</v>
@@ -3203,8 +3283,9 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
-        <v>18</v>
+      <c r="A110" s="7">
+        <f>IF(ROW($A81) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A81)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46568</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>18</v>
@@ -3223,8 +3304,9 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>18</v>
+      <c r="A111" s="7">
+        <f>IF(ROW($A82) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A82)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46598</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>18</v>
@@ -3243,8 +3325,9 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
-        <v>18</v>
+      <c r="A112" s="7">
+        <f>IF(ROW($A83) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A83)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46630</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>18</v>
@@ -3263,8 +3346,9 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
-        <v>18</v>
+      <c r="A113" s="7">
+        <f>IF(ROW($A84) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A84)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v>46660</v>
       </c>
       <c r="B113" s="9" t="s">
         <v>18</v>
@@ -3283,8 +3367,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>18</v>
+      <c r="A114" s="7" t="str">
+        <f>IF(ROW($A85) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A85)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B114" s="9" t="s">
         <v>18</v>
@@ -3303,8 +3388,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>18</v>
+      <c r="A115" s="7" t="str">
+        <f>IF(ROW($A86) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A86)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B115" s="9" t="s">
         <v>18</v>
@@ -3323,8 +3409,9 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
-        <v>18</v>
+      <c r="A116" s="7" t="str">
+        <f>IF(ROW($A87) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A87)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B116" s="9" t="s">
         <v>18</v>
@@ -3343,8 +3430,9 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
-        <v>18</v>
+      <c r="A117" s="7" t="str">
+        <f>IF(ROW($A88) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A88)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B117" s="9" t="s">
         <v>18</v>
@@ -3363,8 +3451,9 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>18</v>
+      <c r="A118" s="7" t="str">
+        <f>IF(ROW($A89) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A89)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B118" s="9" t="s">
         <v>18</v>
@@ -3383,8 +3472,9 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>18</v>
+      <c r="A119" s="7" t="str">
+        <f>IF(ROW($A90) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A90)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B119" s="9" t="s">
         <v>18</v>
@@ -3403,8 +3493,9 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>18</v>
+      <c r="A120" s="7" t="str">
+        <f>IF(ROW($A91) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A91)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B120" s="9" t="s">
         <v>18</v>
@@ -3423,8 +3514,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
-        <v>18</v>
+      <c r="A121" s="7" t="str">
+        <f>IF(ROW($A92) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A92)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B121" s="9" t="s">
         <v>18</v>
@@ -3443,8 +3535,9 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
-        <v>18</v>
+      <c r="A122" s="7" t="str">
+        <f>IF(ROW($A93) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A93)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B122" s="9" t="s">
         <v>18</v>
@@ -3463,8 +3556,9 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
-        <v>18</v>
+      <c r="A123" s="7" t="str">
+        <f>IF(ROW($A94) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A94)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B123" s="9" t="s">
         <v>18</v>
@@ -3483,8 +3577,9 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
-        <v>18</v>
+      <c r="A124" s="7" t="str">
+        <f>IF(ROW($A95) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A95)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B124" s="9" t="s">
         <v>18</v>
@@ -3503,8 +3598,9 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
-        <v>18</v>
+      <c r="A125" s="7" t="str">
+        <f>IF(ROW($A96) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A96)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B125" s="9" t="s">
         <v>18</v>
@@ -3523,8 +3619,9 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="7" t="s">
-        <v>18</v>
+      <c r="A126" s="7" t="str">
+        <f>IF(ROW($A97) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A97)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B126" s="9" t="s">
         <v>18</v>
@@ -3543,8 +3640,9 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
-        <v>18</v>
+      <c r="A127" s="7" t="str">
+        <f>IF(ROW($A98) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A98)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B127" s="9" t="s">
         <v>18</v>
@@ -3563,8 +3661,9 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="7" t="s">
-        <v>18</v>
+      <c r="A128" s="7" t="str">
+        <f>IF(ROW($A99) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A99)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B128" s="9" t="s">
         <v>18</v>
@@ -3583,8 +3682,9 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="7" t="s">
-        <v>18</v>
+      <c r="A129" s="7" t="str">
+        <f>IF(ROW($A100) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A100)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B129" s="9" t="s">
         <v>18</v>
@@ -3603,8 +3703,9 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="7" t="s">
-        <v>18</v>
+      <c r="A130" s="7" t="str">
+        <f>IF(ROW($A101) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A101)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B130" s="9" t="s">
         <v>18</v>
@@ -3623,8 +3724,9 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="7" t="s">
-        <v>18</v>
+      <c r="A131" s="7" t="str">
+        <f>IF(ROW($A102) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A102)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B131" s="9" t="s">
         <v>18</v>
@@ -3643,8 +3745,9 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
-        <v>18</v>
+      <c r="A132" s="7" t="str">
+        <f>IF(ROW($A103) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A103)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B132" s="9" t="s">
         <v>18</v>
@@ -3663,8 +3766,9 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
-        <v>18</v>
+      <c r="A133" s="7" t="str">
+        <f>IF(ROW($A104) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A104)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B133" s="9" t="s">
         <v>18</v>
@@ -3683,8 +3787,9 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="7" t="s">
-        <v>18</v>
+      <c r="A134" s="7" t="str">
+        <f>IF(ROW($A105) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A105)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B134" s="9" t="s">
         <v>18</v>
@@ -3703,8 +3808,9 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
-        <v>18</v>
+      <c r="A135" s="7" t="str">
+        <f>IF(ROW($A106) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A106)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B135" s="9" t="s">
         <v>18</v>
@@ -3723,8 +3829,9 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="7" t="s">
-        <v>18</v>
+      <c r="A136" s="7" t="str">
+        <f>IF(ROW($A107) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A107)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B136" s="9" t="s">
         <v>18</v>
@@ -3743,8 +3850,9 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
-        <v>18</v>
+      <c r="A137" s="7" t="str">
+        <f>IF(ROW($A108) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A108)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B137" s="9" t="s">
         <v>18</v>
@@ -3763,8 +3871,9 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="7" t="s">
-        <v>18</v>
+      <c r="A138" s="7" t="str">
+        <f>IF(ROW($A109) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A109)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B138" s="9" t="s">
         <v>18</v>
@@ -3783,8 +3892,9 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
-        <v>18</v>
+      <c r="A139" s="7" t="str">
+        <f>IF(ROW($A110) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A110)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B139" s="9" t="s">
         <v>18</v>
@@ -3803,8 +3913,9 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="7" t="s">
-        <v>18</v>
+      <c r="A140" s="7" t="str">
+        <f>IF(ROW($A111) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A111)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B140" s="9" t="s">
         <v>18</v>
@@ -3823,8 +3934,9 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
-        <v>18</v>
+      <c r="A141" s="7" t="str">
+        <f>IF(ROW($A112) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A112)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B141" s="9" t="s">
         <v>18</v>
@@ -3843,8 +3955,9 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="7" t="s">
-        <v>18</v>
+      <c r="A142" s="7" t="str">
+        <f>IF(ROW($A113) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A113)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B142" s="9" t="s">
         <v>18</v>
@@ -3863,8 +3976,9 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
-        <v>18</v>
+      <c r="A143" s="7" t="str">
+        <f>IF(ROW($A114) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A114)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B143" s="9" t="s">
         <v>18</v>
@@ -3883,8 +3997,9 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="7" t="s">
-        <v>18</v>
+      <c r="A144" s="7" t="str">
+        <f>IF(ROW($A115) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A115)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B144" s="9" t="s">
         <v>18</v>
@@ -3903,8 +4018,9 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
-        <v>18</v>
+      <c r="A145" s="7" t="str">
+        <f>IF(ROW($A116) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A116)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B145" s="9" t="s">
         <v>18</v>
@@ -3923,8 +4039,9 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="7" t="s">
-        <v>18</v>
+      <c r="A146" s="7" t="str">
+        <f>IF(ROW($A117) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A117)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B146" s="9" t="s">
         <v>18</v>
@@ -3943,8 +4060,9 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="7" t="s">
-        <v>18</v>
+      <c r="A147" s="7" t="str">
+        <f>IF(ROW($A118) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A118)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B147" s="9" t="s">
         <v>18</v>
@@ -3963,8 +4081,9 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="7" t="s">
-        <v>18</v>
+      <c r="A148" s="7" t="str">
+        <f>IF(ROW($A119) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A119)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B148" s="9" t="s">
         <v>18</v>
@@ -3983,8 +4102,9 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="7" t="s">
-        <v>18</v>
+      <c r="A149" s="7" t="str">
+        <f>IF(ROW($A120) &lt;= MonthsCounter,  WORKDAY(EOMONTH(EDATE(fpdate, ROW($A120)), 0) +1, -1, Holiday!$A$1:$A$197), "")</f>
+        <v/>
       </c>
       <c r="B149" s="9" t="s">
         <v>18</v>
@@ -4409,6 +4529,12 @@
     <mergeCell ref="B23:C23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21 F21" xr:uid="{72654645-AAA7-DC4F-8383-7B221AB2A222}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4418,7 +4544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B772"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update both npv datatable
</commit_message>
<xml_diff>
--- a/semester01/COMP7802B Introduction to financial computing/Assignment 1/Darasirikul_Varis_2020_Assignment 1_Question.xlsx
+++ b/semester01/COMP7802B Introduction to financial computing/Assignment 1/Darasirikul_Varis_2020_Assignment 1_Question.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6065D7B4-324D-244B-941D-4F832F6D06CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C3BEE7-7764-E648-B559-2D1FD7FE73DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29940" yWindow="-1740" windowWidth="33540" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,6 +52,16 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -904,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1220,7 @@
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="18">
-        <v>4.9821098788103674E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1220,7 +1230,7 @@
       </c>
       <c r="D24" s="9">
         <f ca="1">B26-F26</f>
-        <v>1.6926787793636322E-7</v>
+        <v>-441.86778471735306</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
@@ -1239,7 +1249,7 @@
       </c>
       <c r="B26" s="9">
         <f ca="1">SUM(C30:C149) - F16</f>
-        <v>63151.115962365642</v>
+        <v>62709.248177479021</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>15</v>
@@ -1251,9 +1261,11 @@
         <v>13</v>
       </c>
       <c r="J26" s="10">
-        <v>63151.115962365642</v>
+        <f ca="1">B26</f>
+        <v>62709.248177479021</v>
       </c>
       <c r="K26" s="10">
+        <f>F26</f>
         <v>63151.115962196374</v>
       </c>
     </row>
@@ -1262,10 +1274,11 @@
         <v>0</v>
       </c>
       <c r="J27" s="9">
+        <f t="dataTable" ref="J27:K62" dt2D="0" dtr="0" r1="D23" ca="1"/>
         <v>200000</v>
       </c>
       <c r="K27" s="9">
-        <v>415000</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1278,7 +1291,7 @@
         <v>193927.86938671139</v>
       </c>
       <c r="K28" s="9">
-        <v>398217.30830456223</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1309,7 +1322,7 @@
         <v>187908.33866143064</v>
       </c>
       <c r="K29" s="9">
-        <v>381687.09724572627</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1322,12 +1335,12 @@
         <v>44134</v>
       </c>
       <c r="B30" s="9">
-        <f>IF(ROW($B1) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" ref="B30:B61" si="0">IF(ROW($B1) &lt;= MonthsCounter, Monthly1, "")</f>
         <v>20000</v>
       </c>
       <c r="C30" s="9">
-        <f ca="1">IF(ROW($C1) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19920.236573710612</v>
+        <f t="shared" ref="C30:C61" ca="1" si="1">IF(ROW($C1) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <v>19919.957588728907</v>
       </c>
       <c r="D30">
         <f>MonthsCounter</f>
@@ -1349,7 +1362,7 @@
         <v>181940.81520699663</v>
       </c>
       <c r="K30" s="9">
-        <v>365404.9947186464</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1362,12 +1375,12 @@
         <v>44165</v>
       </c>
       <c r="B31" s="9">
-        <f>IF(ROW($B2) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C31" s="9">
-        <f ca="1">IF(ROW($C2) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19838.148544168536</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19837.58361641804</v>
       </c>
       <c r="E31" s="7">
         <v>44165</v>
@@ -1385,7 +1398,7 @@
         <v>176024.71446540649</v>
       </c>
       <c r="K31" s="9">
-        <v>349366.71344400477</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1398,12 +1411,12 @@
         <v>44196</v>
       </c>
       <c r="B32" s="9">
-        <f>IF(ROW($B3) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C32" s="9">
-        <f ca="1">IF(ROW($C3) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19756.398785940117</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19755.550280942571</v>
       </c>
       <c r="E32" s="7">
         <v>44196</v>
@@ -1421,7 +1434,7 @@
         <v>170159.45981047861</v>
       </c>
       <c r="K32" s="9">
-        <v>333568.0491516809</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1434,12 +1447,12 @@
         <v>44225</v>
       </c>
       <c r="B33" s="9">
-        <f>IF(ROW($B4) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C33" s="9">
-        <f ca="1">IF(ROW($C4) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19680.228210135112</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19679.116551734962</v>
       </c>
       <c r="E33" s="7">
         <v>44225</v>
@@ -1457,7 +1470,7 @@
         <v>164344.48242281238</v>
       </c>
       <c r="K33" s="9">
-        <v>318004.87880690349</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1470,12 +1483,12 @@
         <v>44253</v>
       </c>
       <c r="B34" s="9">
-        <f>IF(ROW($B5) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C34" s="9">
-        <f ca="1">IF(ROW($C5) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19606.962877601196</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19605.599080980035</v>
       </c>
       <c r="E34" s="7">
         <v>44253</v>
@@ -1493,7 +1506,7 @@
         <v>158579.22116697649</v>
       </c>
       <c r="K34" s="9">
-        <v>302673.15887779277</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1506,12 +1519,12 @@
         <v>44286</v>
       </c>
       <c r="B35" s="9">
-        <f>IF(ROW($B6) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C35" s="9">
-        <f ca="1">IF(ROW($C6) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19520.964530789821</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19519.306004613929</v>
       </c>
       <c r="E35" s="7">
         <v>44286</v>
@@ -1529,7 +1542,7 @@
         <v>152863.12247089134</v>
       </c>
       <c r="K35" s="9">
-        <v>287568.92364326259</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1542,12 +1555,12 @@
         <v>44316</v>
       </c>
       <c r="B36" s="9">
-        <f>IF(ROW($B7) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C36" s="9">
-        <f ca="1">IF(ROW($C7) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19443.111580017347</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19441.187388666553</v>
       </c>
       <c r="E36" s="7">
         <v>44316</v>
@@ -1565,7 +1578,7 @@
         <v>147195.64020735538</v>
       </c>
       <c r="K36" s="9">
-        <v>272688.28354025143</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1578,12 +1591,12 @@
         <v>44347</v>
       </c>
       <c r="B37" s="9">
-        <f>IF(ROW($B8) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C37" s="9">
-        <f ca="1">IF(ROW($C8) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19362.989704362684</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19360.793250048981</v>
       </c>
       <c r="E37" s="7">
         <v>44347</v>
@@ -1601,7 +1614,7 @@
         <v>141576.23557768366</v>
       </c>
       <c r="K37" s="9">
-        <v>258027.42354929773</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1614,12 +1627,12 @@
         <v>44377</v>
       </c>
       <c r="B38" s="9">
-        <f>IF(ROW($B9) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C38" s="9">
-        <f ca="1">IF(ROW($C9) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19285.766784261377</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19283.309021256231</v>
       </c>
       <c r="E38" s="7">
         <v>44377</v>
@@ -1637,7 +1650,7 @@
         <v>136004.3769974045</v>
       </c>
       <c r="K38" s="9">
-        <v>243582.60161749762</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1650,12 +1663,12 @@
         <v>44407</v>
       </c>
       <c r="B39" s="9">
-        <f>IF(ROW($B10) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C39" s="9">
-        <f ca="1">IF(ROW($C10) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19208.851842394837</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19206.134893688883</v>
       </c>
       <c r="E39" s="7">
         <v>44407</v>
@@ -1673,7 +1686,7 @@
         <v>130479.53998397873</v>
       </c>
       <c r="K39" s="9">
-        <v>229350.1471178988</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1686,12 +1699,12 @@
         <v>44439</v>
       </c>
       <c r="B40" s="9">
-        <f>IF(ROW($B11) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C40" s="9">
-        <f ca="1">IF(ROW($C11) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19127.147314372094</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19124.156226513809</v>
       </c>
       <c r="E40" s="7">
         <v>44439</v>
@@ -1709,7 +1722,7 @@
         <v>125001.20704650669</v>
       </c>
       <c r="K40" s="9">
-        <v>215326.45934443153</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1722,12 +1735,12 @@
         <v>44469</v>
       </c>
       <c r="B41" s="9">
-        <f>IF(ROW($B12) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C41" s="9">
-        <f ca="1">IF(ROW($C12) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>19050.864974125281</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>19047.619047619046</v>
       </c>
       <c r="E41" s="7">
         <v>44469</v>
@@ -1745,7 +1758,7 @@
         <v>119568.86757737421</v>
       </c>
       <c r="K41" s="9">
-        <v>201508.00604147511</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1758,12 +1771,12 @@
         <v>44498</v>
       </c>
       <c r="B42" s="9">
-        <f>IF(ROW($B13) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C42" s="9">
-        <f ca="1">IF(ROW($C13) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18977.414576085372</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18973.924286621183</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="7">
@@ -1782,7 +1795,7 @@
         <v>114182.01774580544</v>
       </c>
       <c r="K42" s="9">
-        <v>187891.32196720643</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1795,12 +1808,12 @@
         <v>44530</v>
       </c>
       <c r="B43" s="9">
-        <f>IF(ROW($B14) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C43" s="9">
-        <f ca="1">IF(ROW($C14) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18896.694462579737</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18892.936777540988</v>
       </c>
       <c r="E43" s="7">
         <v>44530</v>
@@ -1818,7 +1831,7 @@
         <v>108840.160393283</v>
       </c>
       <c r="K43" s="9">
-        <v>174473.00748988288</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1831,12 +1844,12 @@
         <v>44561</v>
       </c>
       <c r="B44" s="9">
-        <f>IF(ROW($B15) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C44" s="9">
-        <f ca="1">IF(ROW($C15) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18818.824282295889</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18814.809791373875</v>
       </c>
       <c r="E44" s="7">
         <v>44561</v>
@@ -1854,7 +1867,7 @@
         <v>103542.80493080406</v>
       </c>
       <c r="K44" s="9">
-        <v>161249.72721624677</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -1867,12 +1880,12 @@
         <v>44592</v>
       </c>
       <c r="B45" s="9">
-        <f>IF(ROW($B16) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C45" s="9">
-        <f ca="1">IF(ROW($C16) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18741.2749922603</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18737.005879699595</v>
       </c>
       <c r="E45" s="7">
         <v>44592</v>
@@ -1890,7 +1903,7 @@
         <v>98289.467237923294</v>
       </c>
       <c r="K45" s="9">
-        <v>148218.20865125232</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -1903,12 +1916,12 @@
         <v>44620</v>
       </c>
       <c r="B46" s="9">
-        <f>IF(ROW($B17) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C46" s="9">
-        <f ca="1">IF(ROW($C17) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18671.505184219641</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18667.007956867314</v>
       </c>
       <c r="E46" s="7">
         <v>44620</v>
@@ -1926,7 +1939,7 @@
         <v>93079.669563569129</v>
       </c>
       <c r="K46" s="9">
-        <v>135375.240888339</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -1939,12 +1952,12 @@
         <v>44651</v>
       </c>
       <c r="B47" s="9">
-        <f>IF(ROW($B18) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C47" s="9">
-        <f ca="1">IF(ROW($C18) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18594.562972038286</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18589.815242489458</v>
       </c>
       <c r="E47" s="7">
         <v>44651</v>
@@ -1962,7 +1975,7 @@
         <v>87912.940428571543</v>
       </c>
       <c r="K47" s="9">
-        <v>122717.67332949885</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -1975,12 +1988,12 @@
         <v>44680</v>
       </c>
       <c r="B48" s="9">
-        <f>IF(ROW($B19) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C48" s="9">
-        <f ca="1">IF(ROW($C19) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18522.871841292814</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18517.891712946752</v>
       </c>
       <c r="E48" s="7">
         <v>44680</v>
@@ -1998,7 +2011,7 @@
         <v>82788.814529896015</v>
       </c>
       <c r="K48" s="9">
-        <v>110242.41443440551</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2011,12 +2024,12 @@
         <v>44712</v>
       </c>
       <c r="B49" s="9">
-        <f>IF(ROW($B20) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C49" s="9">
-        <f ca="1">IF(ROW($C20) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18444.085117659575</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18438.850714332362</v>
       </c>
       <c r="E49" s="7">
         <v>44712</v>
@@ -2034,7 +2047,7 @@
         <v>77706.832646529423</v>
       </c>
       <c r="K49" s="9">
-        <v>97946.430497882422</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2047,12 +2060,12 @@
         <v>44742</v>
       </c>
       <c r="B50" s="9">
-        <f>IF(ROW($B21) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C50" s="9">
-        <f ca="1">IF(ROW($C21) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18370.526946471691</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18365.05621072022</v>
       </c>
       <c r="E50" s="7">
         <v>44742</v>
@@ -2070,7 +2083,7 @@
         <v>72666.541546997614</v>
       </c>
       <c r="K50" s="9">
-        <v>85826.744455023902</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2083,12 +2096,12 @@
         <v>44771</v>
       </c>
       <c r="B51" s="9">
-        <f>IF(ROW($B22) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C51" s="9">
-        <f ca="1">IF(ROW($C22) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18299.699584131246</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18294.002268241748</v>
       </c>
       <c r="E51" s="7">
         <v>44771</v>
@@ -2106,7 +2119,7 @@
         <v>67667.493898478104</v>
       </c>
       <c r="K51" s="9">
-        <v>73880.434713285184</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2119,12 +2132,12 @@
         <v>44804</v>
       </c>
       <c r="B52" s="9">
-        <f>IF(ROW($B23) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C52" s="9">
-        <f ca="1">IF(ROW($C23) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18219.43504131529</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18213.482120489338</v>
       </c>
       <c r="E52" s="7">
         <v>44804</v>
@@ -2142,7 +2155,7 @@
         <v>62709.248177479021</v>
       </c>
       <c r="K52" s="9">
-        <v>62104.63401088235</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2155,12 +2168,12 @@
         <v>44834</v>
       </c>
       <c r="B53" s="9">
-        <f>IF(ROW($B24) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C53" s="9">
-        <f ca="1">IF(ROW($C24) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18146.772813117674</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18140.589569160999</v>
       </c>
       <c r="E53" s="7">
         <v>44834</v>
@@ -2178,7 +2191,7 @@
         <v>57791.368582051946</v>
       </c>
       <c r="K53" s="9">
-        <v>50496.528300863458</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2191,12 +2204,12 @@
         <v>44865</v>
       </c>
       <c r="B54" s="9">
-        <f>IF(ROW($B25) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C54" s="9">
-        <f ca="1">IF(ROW($C25) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>18071.992937022103</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>18065.573725567112</v>
       </c>
       <c r="E54" s="7">
         <v>44865</v>
@@ -2214,7 +2227,7 @@
         <v>52913.424945514882</v>
       </c>
       <c r="K54" s="9">
-        <v>39053.355660220608</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2227,12 +2240,12 @@
         <v>44895</v>
       </c>
       <c r="B55" s="9">
-        <f>IF(ROW($B26) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C55" s="9">
-        <f ca="1">IF(ROW($C26) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17999.918733195376</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17993.27312146761</v>
       </c>
       <c r="E55" s="7">
         <v>44895</v>
@@ -2250,7 +2263,7 @@
         <v>48074.992651649867</v>
       </c>
       <c r="K55" s="9">
-        <v>27772.405223438749</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2263,12 +2276,12 @@
         <v>44925</v>
       </c>
       <c r="B56" s="9">
-        <f>IF(ROW($B27) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C56" s="9">
-        <f ca="1">IF(ROW($C27) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17928.131973640866</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17921.261873102532</v>
       </c>
       <c r="E56" s="7">
         <v>44925</v>
@@ -2286,7 +2299,7 @@
         <v>43275.652551348321</v>
       </c>
       <c r="K56" s="9">
-        <v>16651.016139884247</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2299,12 +2312,12 @@
         <v>44957</v>
       </c>
       <c r="B57" s="9">
-        <f>IF(ROW($B28) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C57" s="9">
-        <f ca="1">IF(ROW($C28) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17851.874966025091</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17844.7675044758</v>
       </c>
       <c r="E57" s="7">
         <v>44957</v>
@@ -2322,7 +2335,7 @@
         <v>38514.990880681667</v>
       </c>
       <c r="K57" s="9">
-        <v>5686.5765544563765</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -2335,12 +2348,12 @@
         <v>44985</v>
       </c>
       <c r="B58" s="9">
-        <f>IF(ROW($B29) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C58" s="9">
-        <f ca="1">IF(ROW($C29) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17785.416206412432</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17778.102816064107</v>
       </c>
       <c r="E58" s="7">
         <v>44985</v>
@@ -2358,7 +2371,7 @@
         <v>33792.59918036242</v>
       </c>
       <c r="K58" s="9">
-        <v>-5123.4773890585639</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2371,12 +2384,12 @@
         <v>45016</v>
       </c>
       <c r="B59" s="9">
-        <f>IF(ROW($B30) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C59" s="9">
-        <f ca="1">IF(ROW($C30) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17712.125421658555</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17704.585945228053</v>
       </c>
       <c r="E59" s="7">
         <v>45016</v>
@@ -2394,7 +2407,7 @@
         <v>29108.074216575711</v>
       </c>
       <c r="K59" s="9">
-        <v>-15781.662522480125</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2407,12 +2420,12 @@
         <v>45044</v>
       </c>
       <c r="B60" s="9">
-        <f>IF(ROW($B31) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C60" s="9">
-        <f ca="1">IF(ROW($C31) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17646.186920080007</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17638.444948703407</v>
       </c>
       <c r="E60" s="7">
         <v>45044</v>
@@ -2430,7 +2443,7 @@
         <v>24461.017903155065</v>
       </c>
       <c r="K60" s="9">
-        <v>-26290.449606106151</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -2443,12 +2456,12 @@
         <v>45077</v>
       </c>
       <c r="B61" s="9">
-        <f>IF(ROW($B32) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="C61" s="9">
-        <f ca="1">IF(ROW($C32) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17568.78875739031</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>17560.810204126057</v>
       </c>
       <c r="E61" s="7">
         <v>45077</v>
@@ -2466,7 +2479,7 @@
         <v>19851.037225064822</v>
       </c>
       <c r="K61" s="9">
-        <v>-36652.264260489494</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -2479,12 +2492,12 @@
         <v>45107</v>
       </c>
       <c r="B62" s="9">
-        <f>IF(ROW($B33) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" ref="B62:B93" si="2">IF(ROW($B33) &lt;= MonthsCounter, Monthly1, "")</f>
         <v>20000</v>
       </c>
       <c r="C62" s="9">
-        <f ca="1">IF(ROW($C33) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17498.721418038112</v>
+        <f t="shared" ref="C62:C93" ca="1" si="3">IF(ROW($C33) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <v>17490.529724495449</v>
       </c>
       <c r="E62" s="7">
         <v>45107</v>
@@ -2502,7 +2515,7 @@
         <v>15277.744163188851</v>
       </c>
       <c r="K62" s="9">
-        <v>-46869.487877615262</v>
+        <v>63151.115962196374</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -2515,12 +2528,12 @@
         <v>45138</v>
       </c>
       <c r="B63" s="9">
-        <f>IF(ROW($B34) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C63" s="9">
-        <f ca="1">IF(ROW($C34) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17426.612055511352</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17418.202039819895</v>
       </c>
       <c r="E63" s="7">
         <v>45138</v>
@@ -2542,12 +2555,12 @@
         <v>45169</v>
       </c>
       <c r="B64" s="9">
-        <f>IF(ROW($B35) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C64" s="9">
-        <f ca="1">IF(ROW($C35) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17354.79984384721</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17346.173448085083</v>
       </c>
       <c r="E64" s="7">
         <v>45169</v>
@@ -2569,12 +2582,12 @@
         <v>45198</v>
       </c>
       <c r="B65" s="9">
-        <f>IF(ROW($B36) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C65" s="9">
-        <f ca="1">IF(ROW($C36) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17287.888606054865</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17279.061537494668</v>
       </c>
       <c r="E65" s="7">
         <v>45198</v>
@@ -2596,12 +2609,12 @@
         <v>45230</v>
       </c>
       <c r="B66" s="9">
-        <f>IF(ROW($B37) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C66" s="9">
-        <f ca="1">IF(ROW($C37) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17214.354862827691</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17205.308310063916</v>
       </c>
       <c r="E66" s="7">
         <v>45230</v>
@@ -2623,12 +2636,12 @@
         <v>45260</v>
       </c>
       <c r="B67" s="9">
-        <f>IF(ROW($B38) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C67" s="9">
-        <f ca="1">IF(ROW($C38) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17145.701066566668</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17136.450591873912</v>
       </c>
       <c r="E67" s="7">
         <v>45260</v>
@@ -2650,12 +2663,12 @@
         <v>45289</v>
       </c>
       <c r="B68" s="9">
-        <f>IF(ROW($B39) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C68" s="9">
-        <f ca="1">IF(ROW($C39) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17079.596006784701</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>17070.150093761124</v>
       </c>
       <c r="E68" s="7">
         <v>45289</v>
@@ -2677,12 +2690,12 @@
         <v>45322</v>
       </c>
       <c r="B69" s="9">
-        <f>IF(ROW($B40) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C69" s="9">
-        <f ca="1">IF(ROW($C40) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>17004.682975635569</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16995.016670929337</v>
       </c>
       <c r="E69" s="7">
         <v>45322</v>
@@ -2704,12 +2717,12 @@
         <v>45351</v>
       </c>
       <c r="B70" s="9">
-        <f>IF(ROW($B41) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C70" s="9">
-        <f ca="1">IF(ROW($C41) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16939.121609534905</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16929.263377114097</v>
       </c>
       <c r="E70" s="7">
         <v>45351</v>
@@ -2731,12 +2744,12 @@
         <v>45379</v>
       </c>
       <c r="B71" s="9">
-        <f>IF(ROW($B42) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C71" s="9">
-        <f ca="1">IF(ROW($C42) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16876.060837865811</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16866.01883958836</v>
       </c>
       <c r="E71" s="7">
         <v>45379</v>
@@ -2758,12 +2771,12 @@
         <v>45412</v>
       </c>
       <c r="B72" s="9">
-        <f>IF(ROW($B43) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C72" s="9">
-        <f ca="1">IF(ROW($C43) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16802.040534884432</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16791.783890393228</v>
       </c>
       <c r="E72" s="7">
         <v>45412</v>
@@ -2785,12 +2798,12 @@
         <v>45443</v>
       </c>
       <c r="B73" s="9">
-        <f>IF(ROW($B44) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C73" s="9">
-        <f ca="1">IF(ROW($C44) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16732.802080075369</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16722.345693294857</v>
       </c>
       <c r="E73" s="7">
         <v>45443</v>
@@ -2812,12 +2825,12 @@
         <v>45471</v>
       </c>
       <c r="B74" s="9">
-        <f>IF(ROW($B45) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C74" s="9">
-        <f ca="1">IF(ROW($C45) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16670.509392433181</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16659.874161240627</v>
       </c>
       <c r="E74" s="7">
         <v>45471</v>
@@ -2839,12 +2852,12 @@
         <v>45504</v>
       </c>
       <c r="B75" s="9">
-        <f>IF(ROW($B46) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C75" s="9">
-        <f ca="1">IF(ROW($C46) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16597.390661235371</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16586.546547669244</v>
       </c>
       <c r="E75" s="7">
         <v>45504</v>
@@ -2866,12 +2879,12 @@
         <v>45534</v>
       </c>
       <c r="B76" s="9">
-        <f>IF(ROW($B47) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C76" s="9">
-        <f ca="1">IF(ROW($C47) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16531.197423905189</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16520.165188652463</v>
       </c>
       <c r="E76" s="7">
         <v>45534</v>
@@ -2893,12 +2906,12 @@
         <v>45565</v>
       </c>
       <c r="B77" s="9">
-        <f>IF(ROW($B48) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C77" s="9">
-        <f ca="1">IF(ROW($C48) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16463.075069159146</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16451.850202349931</v>
       </c>
       <c r="E77" s="7">
         <v>45565</v>
@@ -2920,12 +2933,12 @@
         <v>45596</v>
       </c>
       <c r="B78" s="9">
-        <f>IF(ROW($B49) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C78" s="9">
-        <f ca="1">IF(ROW($C49) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16395.233435470211</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16383.817715483707</v>
       </c>
       <c r="E78" s="7">
         <v>45596</v>
@@ -2947,12 +2960,12 @@
         <v>45625</v>
       </c>
       <c r="B79" s="9">
-        <f>IF(ROW($B50) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C79" s="9">
-        <f ca="1">IF(ROW($C50) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16332.021795293869</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16320.429135118013</v>
       </c>
       <c r="E79" s="7">
         <v>45625</v>
@@ -2974,12 +2987,12 @@
         <v>45657</v>
       </c>
       <c r="B80" s="9">
-        <f>IF(ROW($B51) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C80" s="9">
-        <f ca="1">IF(ROW($C51) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16262.553815458832</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16250.76769435296</v>
       </c>
       <c r="E80" s="7">
         <v>45657</v>
@@ -3001,12 +3014,12 @@
         <v>45685</v>
       </c>
       <c r="B81" s="9">
-        <f>IF(ROW($B52) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C81" s="9">
-        <f ca="1">IF(ROW($C52) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16202.011762774371</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16190.057888830241</v>
       </c>
       <c r="E81" s="7">
         <v>45685</v>
@@ -3028,12 +3041,12 @@
         <v>45716</v>
       </c>
       <c r="B82" s="9">
-        <f>IF(ROW($B53) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C82" s="9">
-        <f ca="1">IF(ROW($C53) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16135.245928176861</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16123.107978203901</v>
       </c>
       <c r="E82" s="7">
         <v>45716</v>
@@ -3055,12 +3068,12 @@
         <v>45747</v>
       </c>
       <c r="B83" s="9">
-        <f>IF(ROW($B54) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C83" s="9">
-        <f ca="1">IF(ROW($C54) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16068.755224639292</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>16056.434922086895</v>
       </c>
       <c r="E83" s="7">
         <v>45747</v>
@@ -3082,12 +3095,12 @@
         <v>45777</v>
       </c>
       <c r="B84" s="9">
-        <f>IF(ROW($B55) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C84" s="9">
-        <f ca="1">IF(ROW($C55) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>16004.670275993152</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15992.175133707833</v>
       </c>
       <c r="E84" s="7">
         <v>45777</v>
@@ -3109,12 +3122,12 @@
         <v>45807</v>
       </c>
       <c r="B85" s="9">
-        <f>IF(ROW($B56) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C85" s="9">
-        <f ca="1">IF(ROW($C56) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>15940.840909100894</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15928.172520749258</v>
       </c>
       <c r="E85" s="7">
         <v>45807</v>
@@ -3136,12 +3149,12 @@
         <v>45838</v>
       </c>
       <c r="B86" s="9">
-        <f>IF(ROW($B57) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C86" s="9">
-        <f ca="1">IF(ROW($C57) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>15875.151316779551</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15862.305571166526</v>
       </c>
       <c r="E86" s="7">
         <v>45838</v>
@@ -3163,12 +3176,12 @@
         <v>45869</v>
       </c>
       <c r="B87" s="9">
-        <f>IF(ROW($B58) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C87" s="9">
-        <f ca="1">IF(ROW($C58) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>15809.732420500146</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15796.710997780228</v>
       </c>
       <c r="E87" s="7">
         <v>45869</v>
@@ -3190,12 +3203,12 @@
         <v>45898</v>
       </c>
       <c r="B88" s="9">
-        <f>IF(ROW($B59) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C88" s="9">
-        <f ca="1">IF(ROW($C59) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>15748.778172975568</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15735.59391859971</v>
       </c>
       <c r="E88" s="7">
         <v>45898</v>
@@ -3217,12 +3230,12 @@
         <v>45930</v>
       </c>
       <c r="B89" s="9">
-        <f>IF(ROW($B60) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v>20000</v>
       </c>
       <c r="C89" s="9">
-        <f ca="1">IF(ROW($C60) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
-        <v>15681.791010071955</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15668.428764142789</v>
       </c>
       <c r="E89" s="7">
         <v>45930</v>
@@ -3244,11 +3257,11 @@
         <v/>
       </c>
       <c r="B90" s="9" t="str">
-        <f>IF(ROW($B61) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C90" s="9" t="str">
-        <f ca="1">IF(ROW($A61) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ref="C90:C113" ca="1" si="4">IF(ROW($A61) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
         <v/>
       </c>
       <c r="E90" s="7">
@@ -3271,11 +3284,11 @@
         <v/>
       </c>
       <c r="B91" s="9" t="str">
-        <f>IF(ROW($B62) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C91" s="9" t="str">
-        <f ca="1">IF(ROW($A62) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E91" s="7">
@@ -3298,11 +3311,11 @@
         <v/>
       </c>
       <c r="B92" s="9" t="str">
-        <f>IF(ROW($B63) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C92" s="9" t="str">
-        <f ca="1">IF(ROW($A63) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E92" s="7">
@@ -3325,11 +3338,11 @@
         <v/>
       </c>
       <c r="B93" s="9" t="str">
-        <f>IF(ROW($B64) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="C93" s="9" t="str">
-        <f ca="1">IF(ROW($A64) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E93" s="7">
@@ -3352,11 +3365,11 @@
         <v/>
       </c>
       <c r="B94" s="9" t="str">
-        <f>IF(ROW($B65) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" ref="B94:B125" si="5">IF(ROW($B65) &lt;= MonthsCounter, Monthly1, "")</f>
         <v/>
       </c>
       <c r="C94" s="9" t="str">
-        <f ca="1">IF(ROW($A65) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E94" s="7">
@@ -3379,11 +3392,11 @@
         <v/>
       </c>
       <c r="B95" s="9" t="str">
-        <f>IF(ROW($B66) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C95" s="9" t="str">
-        <f ca="1">IF(ROW($A66) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E95" s="7">
@@ -3406,11 +3419,11 @@
         <v/>
       </c>
       <c r="B96" s="9" t="str">
-        <f>IF(ROW($B67) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C96" s="9" t="str">
-        <f ca="1">IF(ROW($A67) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E96" s="7">
@@ -3433,11 +3446,11 @@
         <v/>
       </c>
       <c r="B97" s="9" t="str">
-        <f>IF(ROW($B68) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C97" s="9" t="str">
-        <f ca="1">IF(ROW($A68) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E97" s="7">
@@ -3460,11 +3473,11 @@
         <v/>
       </c>
       <c r="B98" s="9" t="str">
-        <f>IF(ROW($B69) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C98" s="9" t="str">
-        <f ca="1">IF(ROW($A69) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E98" s="7">
@@ -3487,11 +3500,11 @@
         <v/>
       </c>
       <c r="B99" s="9" t="str">
-        <f>IF(ROW($B70) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C99" s="9" t="str">
-        <f ca="1">IF(ROW($A70) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E99" s="7">
@@ -3514,11 +3527,11 @@
         <v/>
       </c>
       <c r="B100" s="9" t="str">
-        <f>IF(ROW($B71) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C100" s="9" t="str">
-        <f ca="1">IF(ROW($A71) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E100" s="7">
@@ -3541,11 +3554,11 @@
         <v/>
       </c>
       <c r="B101" s="9" t="str">
-        <f>IF(ROW($B72) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C101" s="9" t="str">
-        <f ca="1">IF(ROW($A72) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E101" s="7">
@@ -3568,11 +3581,11 @@
         <v/>
       </c>
       <c r="B102" s="9" t="str">
-        <f>IF(ROW($B73) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C102" s="9" t="str">
-        <f ca="1">IF(ROW($A73) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E102" s="7">
@@ -3595,11 +3608,11 @@
         <v/>
       </c>
       <c r="B103" s="9" t="str">
-        <f>IF(ROW($B74) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C103" s="9" t="str">
-        <f ca="1">IF(ROW($A74) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E103" s="7">
@@ -3622,11 +3635,11 @@
         <v/>
       </c>
       <c r="B104" s="9" t="str">
-        <f>IF(ROW($B75) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C104" s="9" t="str">
-        <f ca="1">IF(ROW($A75) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E104" s="7">
@@ -3649,11 +3662,11 @@
         <v/>
       </c>
       <c r="B105" s="9" t="str">
-        <f>IF(ROW($B76) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C105" s="9" t="str">
-        <f ca="1">IF(ROW($A76) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E105" s="7">
@@ -3676,11 +3689,11 @@
         <v/>
       </c>
       <c r="B106" s="9" t="str">
-        <f>IF(ROW($B77) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C106" s="9" t="str">
-        <f ca="1">IF(ROW($A77) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E106" s="7">
@@ -3703,11 +3716,11 @@
         <v/>
       </c>
       <c r="B107" s="9" t="str">
-        <f>IF(ROW($B78) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C107" s="9" t="str">
-        <f ca="1">IF(ROW($A78) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E107" s="7">
@@ -3730,11 +3743,11 @@
         <v/>
       </c>
       <c r="B108" s="9" t="str">
-        <f>IF(ROW($B79) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C108" s="9" t="str">
-        <f ca="1">IF(ROW($A79) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E108" s="7">
@@ -3757,11 +3770,11 @@
         <v/>
       </c>
       <c r="B109" s="9" t="str">
-        <f>IF(ROW($B80) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C109" s="9" t="str">
-        <f ca="1">IF(ROW($A80) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E109" s="7">
@@ -3784,11 +3797,11 @@
         <v/>
       </c>
       <c r="B110" s="9" t="str">
-        <f>IF(ROW($B81) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C110" s="9" t="str">
-        <f ca="1">IF(ROW($A81) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E110" s="7">
@@ -3811,11 +3824,11 @@
         <v/>
       </c>
       <c r="B111" s="9" t="str">
-        <f>IF(ROW($B82) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C111" s="9" t="str">
-        <f ca="1">IF(ROW($A82) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E111" s="7">
@@ -3838,11 +3851,11 @@
         <v/>
       </c>
       <c r="B112" s="9" t="str">
-        <f>IF(ROW($B83) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C112" s="9" t="str">
-        <f ca="1">IF(ROW($A83) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E112" s="7">
@@ -3865,11 +3878,11 @@
         <v/>
       </c>
       <c r="B113" s="9" t="str">
-        <f>IF(ROW($B84) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C113" s="9" t="str">
-        <f ca="1">IF(ROW($A84) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
       <c r="E113" s="7">
@@ -3892,11 +3905,11 @@
         <v/>
       </c>
       <c r="B114" s="9" t="str">
-        <f>IF(ROW($B85) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C114" s="9" t="str">
-        <f ca="1">IF(ROW($C85) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ref="C114:C149" ca="1" si="6">IF(ROW($C85) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
         <v/>
       </c>
       <c r="E114" s="7" t="s">
@@ -3919,11 +3932,11 @@
         <v/>
       </c>
       <c r="B115" s="9" t="str">
-        <f>IF(ROW($B86) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C115" s="9" t="str">
-        <f ca="1">IF(ROW($C86) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E115" s="7" t="s">
@@ -3946,11 +3959,11 @@
         <v/>
       </c>
       <c r="B116" s="9" t="str">
-        <f>IF(ROW($B87) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C116" s="9" t="str">
-        <f ca="1">IF(ROW($C87) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E116" s="7" t="s">
@@ -3973,11 +3986,11 @@
         <v/>
       </c>
       <c r="B117" s="9" t="str">
-        <f>IF(ROW($B88) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C117" s="9" t="str">
-        <f ca="1">IF(ROW($C88) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E117" s="7" t="s">
@@ -4000,11 +4013,11 @@
         <v/>
       </c>
       <c r="B118" s="9" t="str">
-        <f>IF(ROW($B89) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C118" s="9" t="str">
-        <f ca="1">IF(ROW($C89) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E118" s="7" t="s">
@@ -4027,11 +4040,11 @@
         <v/>
       </c>
       <c r="B119" s="9" t="str">
-        <f>IF(ROW($B90) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C119" s="9" t="str">
-        <f ca="1">IF(ROW($C90) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E119" s="7" t="s">
@@ -4054,11 +4067,11 @@
         <v/>
       </c>
       <c r="B120" s="9" t="str">
-        <f>IF(ROW($B91) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C120" s="9" t="str">
-        <f ca="1">IF(ROW($C91) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E120" s="7" t="s">
@@ -4081,11 +4094,11 @@
         <v/>
       </c>
       <c r="B121" s="9" t="str">
-        <f>IF(ROW($B92) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C121" s="9" t="str">
-        <f ca="1">IF(ROW($C92) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E121" s="7" t="s">
@@ -4108,11 +4121,11 @@
         <v/>
       </c>
       <c r="B122" s="9" t="str">
-        <f>IF(ROW($B93) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C122" s="9" t="str">
-        <f ca="1">IF(ROW($C93) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E122" s="7" t="s">
@@ -4135,11 +4148,11 @@
         <v/>
       </c>
       <c r="B123" s="9" t="str">
-        <f>IF(ROW($B94) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C123" s="9" t="str">
-        <f ca="1">IF(ROW($C94) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E123" s="7" t="s">
@@ -4162,11 +4175,11 @@
         <v/>
       </c>
       <c r="B124" s="9" t="str">
-        <f>IF(ROW($B95) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C124" s="9" t="str">
-        <f ca="1">IF(ROW($C95) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E124" s="7" t="s">
@@ -4189,11 +4202,11 @@
         <v/>
       </c>
       <c r="B125" s="9" t="str">
-        <f>IF(ROW($B96) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C125" s="9" t="str">
-        <f ca="1">IF(ROW($C96) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E125" s="7" t="s">
@@ -4216,11 +4229,11 @@
         <v/>
       </c>
       <c r="B126" s="9" t="str">
-        <f>IF(ROW($B97) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" ref="B126:B157" si="7">IF(ROW($B97) &lt;= MonthsCounter, Monthly1, "")</f>
         <v/>
       </c>
       <c r="C126" s="9" t="str">
-        <f ca="1">IF(ROW($C97) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E126" s="7" t="s">
@@ -4243,11 +4256,11 @@
         <v/>
       </c>
       <c r="B127" s="9" t="str">
-        <f>IF(ROW($B98) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C127" s="9" t="str">
-        <f ca="1">IF(ROW($C98) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E127" s="7" t="s">
@@ -4270,11 +4283,11 @@
         <v/>
       </c>
       <c r="B128" s="9" t="str">
-        <f>IF(ROW($B99) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C128" s="9" t="str">
-        <f ca="1">IF(ROW($C99) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E128" s="7" t="s">
@@ -4297,11 +4310,11 @@
         <v/>
       </c>
       <c r="B129" s="9" t="str">
-        <f>IF(ROW($B100) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C129" s="9" t="str">
-        <f ca="1">IF(ROW($C100) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E129" s="7" t="s">
@@ -4324,11 +4337,11 @@
         <v/>
       </c>
       <c r="B130" s="9" t="str">
-        <f>IF(ROW($B101) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C130" s="9" t="str">
-        <f ca="1">IF(ROW($C101) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E130" s="7" t="s">
@@ -4351,11 +4364,11 @@
         <v/>
       </c>
       <c r="B131" s="9" t="str">
-        <f>IF(ROW($B102) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C131" s="9" t="str">
-        <f ca="1">IF(ROW($C102) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E131" s="7" t="s">
@@ -4378,11 +4391,11 @@
         <v/>
       </c>
       <c r="B132" s="9" t="str">
-        <f>IF(ROW($B103) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C132" s="9" t="str">
-        <f ca="1">IF(ROW($C103) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E132" s="7" t="s">
@@ -4405,11 +4418,11 @@
         <v/>
       </c>
       <c r="B133" s="9" t="str">
-        <f>IF(ROW($B104) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C133" s="9" t="str">
-        <f ca="1">IF(ROW($C104) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E133" s="7" t="s">
@@ -4432,11 +4445,11 @@
         <v/>
       </c>
       <c r="B134" s="9" t="str">
-        <f>IF(ROW($B105) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C134" s="9" t="str">
-        <f ca="1">IF(ROW($C105) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E134" s="7" t="s">
@@ -4459,11 +4472,11 @@
         <v/>
       </c>
       <c r="B135" s="9" t="str">
-        <f>IF(ROW($B106) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C135" s="9" t="str">
-        <f ca="1">IF(ROW($C106) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E135" s="7" t="s">
@@ -4486,11 +4499,11 @@
         <v/>
       </c>
       <c r="B136" s="9" t="str">
-        <f>IF(ROW($B107) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C136" s="9" t="str">
-        <f ca="1">IF(ROW($C107) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E136" s="7" t="s">
@@ -4513,11 +4526,11 @@
         <v/>
       </c>
       <c r="B137" s="9" t="str">
-        <f>IF(ROW($B108) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C137" s="9" t="str">
-        <f ca="1">IF(ROW($C108) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E137" s="7" t="s">
@@ -4540,11 +4553,11 @@
         <v/>
       </c>
       <c r="B138" s="9" t="str">
-        <f>IF(ROW($B109) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C138" s="9" t="str">
-        <f ca="1">IF(ROW($C109) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E138" s="7" t="s">
@@ -4567,11 +4580,11 @@
         <v/>
       </c>
       <c r="B139" s="9" t="str">
-        <f>IF(ROW($B110) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C139" s="9" t="str">
-        <f ca="1">IF(ROW($C110) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E139" s="7" t="s">
@@ -4594,11 +4607,11 @@
         <v/>
       </c>
       <c r="B140" s="9" t="str">
-        <f>IF(ROW($B111) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C140" s="9" t="str">
-        <f ca="1">IF(ROW($C111) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E140" s="7" t="s">
@@ -4621,11 +4634,11 @@
         <v/>
       </c>
       <c r="B141" s="9" t="str">
-        <f>IF(ROW($B112) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C141" s="9" t="str">
-        <f ca="1">IF(ROW($C112) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E141" s="7" t="s">
@@ -4648,11 +4661,11 @@
         <v/>
       </c>
       <c r="B142" s="9" t="str">
-        <f>IF(ROW($B113) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C142" s="9" t="str">
-        <f ca="1">IF(ROW($C113) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E142" s="7" t="s">
@@ -4675,11 +4688,11 @@
         <v/>
       </c>
       <c r="B143" s="9" t="str">
-        <f>IF(ROW($B114) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C143" s="9" t="str">
-        <f ca="1">IF(ROW($C114) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E143" s="7" t="s">
@@ -4702,11 +4715,11 @@
         <v/>
       </c>
       <c r="B144" s="9" t="str">
-        <f>IF(ROW($B115) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C144" s="9" t="str">
-        <f ca="1">IF(ROW($C115) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E144" s="7" t="s">
@@ -4729,11 +4742,11 @@
         <v/>
       </c>
       <c r="B145" s="9" t="str">
-        <f>IF(ROW($B116) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C145" s="9" t="str">
-        <f ca="1">IF(ROW($C116) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E145" s="7" t="s">
@@ -4756,11 +4769,11 @@
         <v/>
       </c>
       <c r="B146" s="9" t="str">
-        <f>IF(ROW($B117) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C146" s="9" t="str">
-        <f ca="1">IF(ROW($C117) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E146" s="7" t="s">
@@ -4783,11 +4796,11 @@
         <v/>
       </c>
       <c r="B147" s="9" t="str">
-        <f>IF(ROW($B118) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C147" s="9" t="str">
-        <f ca="1">IF(ROW($C118) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E147" s="7" t="s">
@@ -4810,11 +4823,11 @@
         <v/>
       </c>
       <c r="B148" s="9" t="str">
-        <f>IF(ROW($B119) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C148" s="9" t="str">
-        <f ca="1">IF(ROW($C119) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E148" s="7" t="s">
@@ -4837,11 +4850,11 @@
         <v/>
       </c>
       <c r="B149" s="9" t="str">
-        <f>IF(ROW($B120) &lt;= MonthsCounter, Monthly1, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C149" s="9" t="str">
-        <f ca="1">IF(ROW($C120) &lt;= MonthsCounter,  INDIRECT("RC[-1]",0) / (POWER( (1 + $D$23), (INDIRECT("RC[-2]",0) - $B$16) / 365)), "")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="E149" s="7" t="s">

</xml_diff>